<commit_message>
Remove mode shifting to rail
</commit_message>
<xml_diff>
--- a/InputData/trans/RTMF/Recipient Transportation Mode Fractions.xlsx
+++ b/InputData/trans/RTMF/Recipient Transportation Mode Fractions.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\RMI\All_states_RMI\OR\trans\RTMF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganM\Documents\eps-oregon\InputData\trans\RTMF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{003EE5AC-58EE-4F1F-8648-4D8046C32E77}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2565" yWindow="3720" windowWidth="13980" windowHeight="12390" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2565" yWindow="3720" windowWidth="13980" windowHeight="12390"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="RTMF-passengers" sheetId="2" r:id="rId2"/>
     <sheet name="RTMF-freight" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -150,7 +149,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -533,17 +532,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="18.7109375" customWidth="1"/>
+    <col min="2" max="2" width="18.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -554,7 +553,7 @@
         <v>44319</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -562,80 +561,80 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A21" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A22" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A23" s="2"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A24" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A25" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A26" s="2"/>
       <c r="B26" s="1" t="s">
         <v>24</v>
@@ -644,7 +643,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A27" s="2"/>
       <c r="B27" s="1" t="s">
         <v>25</v>
@@ -653,7 +652,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A28" s="2"/>
       <c r="B28" s="1" t="s">
         <v>26</v>
@@ -669,24 +668,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="22.3984375" customWidth="1"/>
+    <col min="7" max="7" width="11.59765625" customWidth="1"/>
+    <col min="8" max="8" width="9.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -712,7 +711,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -720,13 +719,13 @@
         <v>0</v>
       </c>
       <c r="C2" s="4">
-        <v>0.15</v>
+        <v>0.2</v>
       </c>
       <c r="D2" s="4">
         <v>0</v>
       </c>
       <c r="E2" s="4">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="F2" s="4">
         <v>0</v>
@@ -739,7 +738,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -767,7 +766,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -795,7 +794,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -823,7 +822,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -851,7 +850,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -879,7 +878,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
@@ -894,24 +893,24 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="22.3984375" customWidth="1"/>
+    <col min="7" max="7" width="11.59765625" customWidth="1"/>
+    <col min="8" max="8" width="9.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -937,7 +936,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -965,7 +964,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -993,7 +992,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -1021,7 +1020,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -1049,7 +1048,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -1077,7 +1076,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -1105,7 +1104,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>

</xml_diff>

<commit_message>
Temporary adjustment for RTMF
</commit_message>
<xml_diff>
--- a/InputData/trans/RTMF/Recipient Transportation Mode Fractions.xlsx
+++ b/InputData/trans/RTMF/Recipient Transportation Mode Fractions.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganM\Documents\eps-us\InputData\trans\RTMF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-oregon\InputData\trans\RTMF\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E77047D8-3793-4D00-B269-54154D697D4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3930" yWindow="2250" windowWidth="23595" windowHeight="14160"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="RTMF-passengers" sheetId="2" r:id="rId2"/>
     <sheet name="RTMF-freight" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -146,7 +147,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -528,22 +529,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="18.73046875" customWidth="1"/>
+    <col min="2" max="2" width="18.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -551,80 +552,80 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="2"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="2"/>
       <c r="B26" s="1" t="s">
         <v>24</v>
@@ -633,7 +634,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="2"/>
       <c r="B27" s="1" t="s">
         <v>25</v>
@@ -642,7 +643,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="2"/>
       <c r="B28" s="1" t="s">
         <v>26</v>
@@ -658,22 +659,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22.3984375" customWidth="1"/>
-    <col min="7" max="7" width="11.59765625" customWidth="1"/>
-    <col min="8" max="8" width="9.1328125" customWidth="1"/>
+    <col min="1" max="1" width="22.36328125" customWidth="1"/>
+    <col min="7" max="7" width="11.6328125" customWidth="1"/>
+    <col min="8" max="8" width="9.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -699,7 +702,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -707,13 +710,13 @@
         <v>0</v>
       </c>
       <c r="C2" s="4">
-        <v>0.33</v>
+        <v>0.2</v>
       </c>
       <c r="D2" s="4">
         <v>0</v>
       </c>
       <c r="E2" s="4">
-        <v>0.33</v>
+        <v>0</v>
       </c>
       <c r="F2" s="4">
         <v>0</v>
@@ -723,11 +726,10 @@
       </c>
       <c r="H2" s="4"/>
       <c r="I2" s="6">
-        <f>1-SUM(B2:G2)</f>
-        <v>0.33999999999999997</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -755,7 +757,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -783,7 +785,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -811,7 +813,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -839,7 +841,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -867,7 +869,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
@@ -882,7 +884,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
@@ -892,14 +894,14 @@
       <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22.3984375" customWidth="1"/>
-    <col min="7" max="7" width="11.59765625" customWidth="1"/>
-    <col min="8" max="8" width="9.1328125" customWidth="1"/>
+    <col min="1" max="1" width="22.36328125" customWidth="1"/>
+    <col min="7" max="7" width="11.6328125" customWidth="1"/>
+    <col min="8" max="8" width="9.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -925,7 +927,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -953,7 +955,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -981,7 +983,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -1009,7 +1011,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -1037,7 +1039,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -1065,7 +1067,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -1093,7 +1095,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>

</xml_diff>